<commit_message>
Update spread sheet with scope to local-def.
</commit_message>
<xml_diff>
--- a/trestle_k8s/Kubernetes-Yaml-to-OSCAL-Mapping.xlsx
+++ b/trestle_k8s/Kubernetes-Yaml-to-OSCAL-Mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="117">
   <si>
     <t xml:space="preserve">Kubernetes Yaml to OSCAL Json mapping</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">2. Use the “path” to the property as the OSCAL property name.</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Put the property into one of: results or obsercation properties.</t>
+    <t xml:space="preserve">3. Put the property into one of: local-definition, results or observation properties.</t>
   </si>
   <si>
     <t xml:space="preserve">Note that XXXXX means property not found in the sample use case.</t>
@@ -67,6 +67,39 @@
     <t xml:space="preserve">rhacm value (example)</t>
   </si>
   <si>
+    <t xml:space="preserve">local-definitions.inventory-items.prop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope.apiVersion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“policy.open-cluster-management.io/v1”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope.kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Policy”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“policy-imagemanifestvuln”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope.namesapce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope.namespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“cluster1”</t>
+  </si>
+  <si>
     <t xml:space="preserve">result.title</t>
   </si>
   <si>
@@ -97,9 +130,6 @@
     <t xml:space="preserve">"kube-cis"</t>
   </si>
   <si>
-    <t xml:space="preserve">XXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXX</t>
-  </si>
-  <si>
     <t xml:space="preserve">metadata.labels.policy.kubernetes.io/engine</t>
   </si>
   <si>
@@ -161,33 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">“v1.5.1 – 02-14-2020”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope.apiVersion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“policy.open-cluster-management.io/v1”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope.kind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Policy”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“policy-imagemanifestvuln”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope.namesapce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope.namespace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“cluster1”</t>
   </si>
   <si>
     <t xml:space="preserve">results.policy</t>
@@ -614,10 +617,10 @@
   <dimension ref="A2:AMJ50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.98"/>
@@ -648,7 +651,7 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -706,391 +709,391 @@
         <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+    <row r="12" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="E15" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>25</v>
-      </c>
+    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="E22" s="8" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+    <row r="24" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="4" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
@@ -1108,525 +1111,525 @@
     </row>
     <row r="27" s="4" customFormat="true" ht="99.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
     </row>
     <row r="34" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
     <row r="35" s="4" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
     <row r="36" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
     <row r="42" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
     <row r="43" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
     <row r="44" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
     <row r="45" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
     <row r="46" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
     <row r="47" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
@@ -1665,17 +1668,17 @@
       <c r="AMJ50" s="0"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A31:D32 D30:G30 A47:A48 A38:G42 D33:F36 A30:C36 A49:G50 E31:G33 G34:G37 A37:F38 G47 B47:F47 B48:G48 B24:G29 B19:C19 E18:G19 A12:A14 B18:C18 B20:G23 A24 A27:A29 B9:G17">
+  <conditionalFormatting sqref="A31:D32 D30:G30 A47:A48 A38:G42 D33:F36 A30:C36 A49:G50 E31:G33 G34:G37 A37:F38 G47 B47:F47 B48:G48 B25:G29 E23:G24 A17:A19 B23:C24 A27:A29 B14:G22 A9:G13">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
+  <conditionalFormatting sqref="D24">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
+  <conditionalFormatting sqref="D23">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
@@ -1705,63 +1708,43 @@
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A14">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A20">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:A11">
+  <conditionalFormatting sqref="A15:A16">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
+  <conditionalFormatting sqref="A21">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
+  <conditionalFormatting sqref="A22">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="A23">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
+  <conditionalFormatting sqref="A24">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
+  <conditionalFormatting sqref="A25:A26">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISODD(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISODD(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISODD(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>ISODD(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A26">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add namespace and class to example.
</commit_message>
<xml_diff>
--- a/trestle_k8s/Kubernetes-Yaml-to-OSCAL-Mapping.xlsx
+++ b/trestle_k8s/Kubernetes-Yaml-to-OSCAL-Mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="122">
   <si>
     <t xml:space="preserve">Kubernetes Yaml to OSCAL Json mapping</t>
   </si>
@@ -37,21 +37,24 @@
     <t xml:space="preserve">3. Put the property into one of: local-definition, results or observation properties.</t>
   </si>
   <si>
+    <t xml:space="preserve">4. Assign property ns and class, if applicable.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Note that XXXXX means property not found in the sample use case.</t>
   </si>
   <si>
     <t xml:space="preserve">Note that ***** means not applicable.</t>
   </si>
   <si>
-    <t xml:space="preserve">Note that mapping to SCC class not attempted.</t>
-  </si>
-  <si>
     <t xml:space="preserve">OSCAL json Path</t>
   </si>
   <si>
     <t xml:space="preserve">property name</t>
   </si>
   <si>
+    <t xml:space="preserve">property class</t>
+  </si>
+  <si>
     <t xml:space="preserve">yaml path</t>
   </si>
   <si>
@@ -94,6 +97,9 @@
     <t xml:space="preserve">scope.namesapce</t>
   </si>
   <si>
+    <t xml:space="preserve">scc_scope</t>
+  </si>
+  <si>
     <t xml:space="preserve">scope.namespace</t>
   </si>
   <si>
@@ -196,6 +202,9 @@
     <t xml:space="preserve">results.policy</t>
   </si>
   <si>
+    <t xml:space="preserve">scc_rule</t>
+  </si>
+  <si>
     <t xml:space="preserve">"api-server:anonymous-auth"</t>
   </si>
   <si>
@@ -214,6 +223,9 @@
     <t xml:space="preserve">results.message</t>
   </si>
   <si>
+    <t xml:space="preserve">scc_description</t>
+  </si>
+  <si>
     <t xml:space="preserve">"ensure that --anonymous-auth argument is set to false"</t>
   </si>
   <si>
@@ -227,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">results.result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scc_result</t>
   </si>
   <si>
     <t xml:space="preserve">"warn"</t>
@@ -616,18 +631,20 @@
   </sheetPr>
   <dimension ref="A2:AMJ50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="29.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.44"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,12 +660,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="AMI4" s="0"/>
+      <c r="C4" s="3"/>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3"/>
-      <c r="AMI5" s="0"/>
+      <c r="C5" s="3"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +687,6 @@
       <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,107 +714,111 @@
       <c r="G8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AMI8" s="0"/>
+      <c r="H8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AMI9" s="0"/>
+      <c r="H9" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AMI10" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AMI11" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="AMI12" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,82 +829,82 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="AMI13" s="0"/>
+      <c r="H13" s="8"/>
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AMI14" s="0"/>
+        <v>33</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
-    </row>
-    <row r="16" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="B16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>36</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AMI16" s="0"/>
+        <v>40</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,743 +915,749 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="AMI17" s="0"/>
+      <c r="H17" s="8"/>
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AMI18" s="0"/>
+        <v>44</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>43</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AMI19" s="0"/>
+        <v>46</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="AMJ19" s="0"/>
     </row>
-    <row r="20" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>45</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI20" s="0"/>
+        <v>48</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI21" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>50</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI22" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ22" s="0"/>
     </row>
-    <row r="23" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI23" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI24" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ24" s="0"/>
     </row>
-    <row r="25" s="4" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="8" t="s">
+    <row r="25" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="AMJ25" s="0"/>
+    </row>
+    <row r="26" s="4" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="D26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AMI25" s="0"/>
-      <c r="AMJ25" s="0"/>
-    </row>
-    <row r="26" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="AMI26" s="0"/>
+      <c r="F26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" s="4" customFormat="true" ht="99.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="AMI27" s="0"/>
+        <v>70</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AMI28" s="0"/>
+        <v>75</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AMI29" s="0"/>
+        <v>78</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>74</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C30" s="8"/>
       <c r="D30" s="8" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI30" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>76</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI31" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>78</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C32" s="8"/>
       <c r="D32" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI32" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>80</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="8" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI33" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ33" s="0"/>
     </row>
-    <row r="34" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>82</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C34" s="8"/>
       <c r="D34" s="8" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI34" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ34" s="0"/>
     </row>
     <row r="35" s="4" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>84</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C35" s="8"/>
       <c r="D35" s="8" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AMI35" s="0"/>
+        <v>90</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>87</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C36" s="8"/>
       <c r="D36" s="8" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI36" s="0"/>
+        <v>93</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>89</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C37" s="8"/>
       <c r="D37" s="8" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI37" s="0"/>
+        <v>95</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>91</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C38" s="8"/>
       <c r="D38" s="8" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMI38" s="0"/>
+        <v>97</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>93</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C39" s="8"/>
       <c r="D39" s="8" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AMI39" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>95</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C40" s="8"/>
       <c r="D40" s="8" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="AMI40" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>97</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C41" s="8"/>
       <c r="D41" s="8" t="s">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="AMI41" s="0"/>
+        <v>18</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="AMJ41" s="0"/>
     </row>
     <row r="42" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>99</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C42" s="8"/>
       <c r="D42" s="8" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AMI42" s="0"/>
+        <v>105</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>102</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C43" s="8"/>
       <c r="D43" s="8" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="AMI43" s="0"/>
+        <v>108</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>105</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C44" s="8"/>
       <c r="D44" s="8" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="AMI44" s="0"/>
+        <v>111</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>108</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C45" s="8"/>
       <c r="D45" s="8" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AMI45" s="0"/>
+        <v>114</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" s="4" customFormat="true" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>111</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C46" s="8"/>
       <c r="D46" s="8" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AMI46" s="0"/>
+        <v>48</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" s="4" customFormat="true" ht="19.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="4" customFormat="true" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C47" s="8"/>
       <c r="D47" s="8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="AMI47" s="0"/>
+        <v>121</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="AMJ47" s="0"/>
     </row>
     <row r="48" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,7 +1668,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="AMI48" s="0"/>
+      <c r="H48" s="8"/>
       <c r="AMJ48" s="0"/>
     </row>
     <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,7 +1679,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="AMI49" s="0"/>
+      <c r="H49" s="8"/>
       <c r="AMJ49" s="0"/>
     </row>
     <row r="50" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,26 +1690,26 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="AMI50" s="0"/>
+      <c r="H50" s="8"/>
       <c r="AMJ50" s="0"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A31:D32 D30:G30 A47:A48 A38:G42 D33:F36 A30:C36 A49:G50 E31:G33 G34:G37 A37:F38 G47 B47:F47 B48:G48 B25:G29 E23:G24 A17:A19 B23:C24 A27:A29 B14:G22 A9:G13">
+  <conditionalFormatting sqref="A31:E32 E30:H30 A47:A48 A38:H42 E33:G36 A30:D36 A49:H50 F31:H33 H34:H37 A37:G38 H47 B47:G47 B48:H48 B26:H29 F23:H25 A17:A19 B23:D25 A27:A29 B14:H22 A9:H13">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
+  <conditionalFormatting sqref="E24:E25">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
+  <conditionalFormatting sqref="E23">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:G46">
+  <conditionalFormatting sqref="B43:H46">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
@@ -1738,12 +1764,12 @@
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
+  <conditionalFormatting sqref="A24:A25">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A26">
+  <conditionalFormatting sqref="A26">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>ISODD(ROW())</formula>
     </cfRule>

</xml_diff>